<commit_message>
Change "Reason" column to "Category" and further curate dataset
</commit_message>
<xml_diff>
--- a/Datasets/Curated-Dataset_2025-04-18.xlsx
+++ b/Datasets/Curated-Dataset_2025-04-18.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="pulumi" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="482">
   <si>
     <t xml:space="preserve">Url</t>
   </si>
@@ -50,7 +50,7 @@
     <t xml:space="preserve">Include</t>
   </si>
   <si>
-    <t xml:space="preserve">Reason</t>
+    <t xml:space="preserve">Category</t>
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
@@ -74,7 +74,25 @@
 Since `Pulumi.Config` is a sealed class, there is no possibility to mock it as well. </t>
   </si>
   <si>
-    <t xml:space="preserve">breaking</t>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">breaking, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">complexity</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Stack Configuration</t>
@@ -151,6 +169,9 @@
 https://github.com/pulumi/pulumi/issues/4472
 https://github.com/pulumi/pulumi/issues/9212
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">breaking, complexity</t>
   </si>
   <si>
     <t xml:space="preserve">Stack Configuration, Stack Reference</t>
@@ -266,7 +287,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Stack Reference</t>
+    <t xml:space="preserve">coverage, complexity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expose Data (Stack Output)</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi/issues/11393</t>
@@ -360,10 +384,25 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">coverage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent-child, Stack Output, post-deployment state</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Expose Data (Stack Output), Resource Relationships (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Parent-child)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi/issues/10533</t>
@@ -382,7 +421,28 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Component resources do not pass their input/output properties to the Pulumi engine.</t>
+    <t xml:space="preserve">coverage</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Expose Data (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Component resources do not pass their input/output properties to the Pulumi engine.)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi/issues/8280</t>
@@ -470,7 +530,25 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Expose additional resource metadata</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Expose Data (more </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">resource metadata)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi/issues/12859</t>
@@ -773,9 +851,6 @@
 2. Asserting resources - currently I have to rewrite my stack in a way that I need to collect all created resources and have them available for the UT. It would be nice if we could pull the created resources by their name from somewhere. It feels "wrong" that I have to rewrite my stack just so it will be testable in this manner.
 WDYT?
 @EvanBoyle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stack Output</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi/issues/4669</t>
@@ -1895,6 +1970,9 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Expose Data (more resource metadata)</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi/issues/7972</t>
   </si>
   <si>
@@ -2164,7 +2242,25 @@
     <t xml:space="preserve">dependsOn is an "option" for any resource, but does not get exposed as a property or anything that we can inspect. We are looking for a way to unit test resources to assert that dependsOn is correct / what we expect</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource dependencies</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Resource Relationships (D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ependencies)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi/issues/3879</t>
@@ -2367,7 +2463,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Assert on CustomResourceOptions</t>
+    <t xml:space="preserve">Expose Data (Assert on CustomResourceOptions)</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi-dotnet/issues/365 </t>
@@ -2541,7 +2637,7 @@
 Pulumi Core</t>
   </si>
   <si>
-    <t xml:space="preserve">Assert on Pulumi-specific exceptions</t>
+    <t xml:space="preserve">Expose Internals (Assert on Pulumi-specific exceptions)</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi-dotnet/issues/134 </t>
@@ -3203,7 +3299,7 @@
 Logging.</t>
   </si>
   <si>
-    <t xml:space="preserve">MAke Pulumi.Log safe to call outside of a Pulumi run</t>
+    <t xml:space="preserve">Expose Internals (Make Pulumi.Log safe to call outside of a Pulumi run)</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi-dotnet/issues/140 </t>
@@ -3270,7 +3366,25 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Support to TestWithServiceProviderAsync() for retrieving stack outputs</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Expose Data (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Stack Output (Support in TestWithServiceProviderAsync()))</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi-dotnet/issues/13 </t>
@@ -3319,7 +3433,7 @@
 How should unit testing work with top level programs? Can it work with top level programs? Do we just need to document this.</t>
   </si>
   <si>
-    <t xml:space="preserve">Support Unit Testing with Top-Level Statements</t>
+    <t xml:space="preserve">Program Style (Support Unit Testing with Top-Level Statements)</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/pulumi/pulumi-dotnet/issues/149 </t>
@@ -3475,6 +3589,9 @@
     <t xml:space="preserve">ProTI does not access stack configuration nor generate its own values for [Pulumi's configuration mechanism](https://www.pulumi.com/docs/concepts/config/). We should add an interface to generator plugins to generate accessed configuration values.</t>
   </si>
   <si>
+    <t xml:space="preserve">breaking</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -3506,7 +3623,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3560,7 +3677,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3580,12 +3697,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3633,7 +3744,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3674,10 +3785,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3699,10 +3806,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3938,8 +4041,8 @@
   </sheetPr>
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="90" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3951,8 +4054,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="255"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="81.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="173.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3977,10 +4080,10 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4033,7 +4136,8 @@
       <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="8" t="b">
+      <c r="G3" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -4064,18 +4168,18 @@
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6" t="n">
         <v>43737.7168287037</v>
@@ -4087,21 +4191,22 @@
         <v>7</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="10" t="b">
+        <v>25</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="n">
         <v>44599.4231134259</v>
@@ -4113,25 +4218,25 @@
         <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" s="6" t="n">
         <v>44882.4800347222</v>
@@ -4143,22 +4248,23 @@
         <v>3</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6" t="n">
         <v>44842.5868055556</v>
@@ -4170,21 +4276,22 @@
         <v>3</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6" t="n">
         <v>44286.625474537</v>
@@ -4196,25 +4303,25 @@
         <v>3</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="6" t="n">
         <v>44803.6903125</v>
@@ -4226,25 +4333,25 @@
         <v>2</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>44491.3134837963</v>
@@ -4256,22 +4363,22 @@
         <v>2</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G11" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" s="6" t="n">
         <v>44385.8107175926</v>
@@ -4283,21 +4390,22 @@
         <v>2</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" s="10" t="b">
+        <v>53</v>
+      </c>
+      <c r="G12" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" s="6" t="n">
         <v>45434.6205555556</v>
@@ -4309,21 +4417,22 @@
         <v>1</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="10" t="b">
+        <v>56</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C14" s="6" t="n">
         <v>45427.2263541667</v>
@@ -4335,21 +4444,22 @@
         <v>1</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="10" t="b">
+        <v>59</v>
+      </c>
+      <c r="G14" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C15" s="6" t="n">
         <v>45225.9921875</v>
@@ -4361,25 +4471,25 @@
         <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G15" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>61</v>
+        <v>46</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C16" s="6" t="n">
         <v>45056.8481481482</v>
@@ -4391,21 +4501,22 @@
         <v>1</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="10" t="b">
+        <v>66</v>
+      </c>
+      <c r="G16" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C17" s="6" t="n">
         <v>44797.0890046296</v>
@@ -4417,21 +4528,22 @@
         <v>1</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G17" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C18" s="6" t="n">
         <v>44643.8319675926</v>
@@ -4443,21 +4555,22 @@
         <v>1</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C19" s="6" t="n">
         <v>44431.6193981481</v>
@@ -4469,21 +4582,22 @@
         <v>1</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G19" s="10" t="b">
+        <v>75</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>44425.6697337963</v>
@@ -4495,21 +4609,22 @@
         <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="10" t="b">
+        <v>78</v>
+      </c>
+      <c r="G20" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C21" s="6" t="n">
         <v>44376.0834953704</v>
@@ -4521,22 +4636,22 @@
         <v>1</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G21" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C22" s="6" t="n">
         <v>44224.8942939815</v>
@@ -4548,21 +4663,22 @@
         <v>1</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="10" t="b">
+        <v>84</v>
+      </c>
+      <c r="G22" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C23" s="6" t="n">
         <v>44210.8715856482</v>
@@ -4574,25 +4690,25 @@
         <v>1</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G23" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>86</v>
+        <v>30</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>43970.7928009259</v>
@@ -4604,22 +4720,22 @@
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G24" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C25" s="6" t="n">
         <v>43846.8824189815</v>
@@ -4631,21 +4747,22 @@
         <v>1</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="10" t="b">
+        <v>93</v>
+      </c>
+      <c r="G25" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>93</v>
+      <c r="A26" s="11" t="s">
+        <v>94</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C26" s="6" t="n">
         <v>45750.674837963</v>
@@ -4657,21 +4774,22 @@
         <v>0</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G26" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C27" s="6" t="n">
         <v>45747.3927430556</v>
@@ -4683,21 +4801,22 @@
         <v>0</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="10" t="b">
+        <v>99</v>
+      </c>
+      <c r="G27" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C28" s="6" t="n">
         <v>45741.3655902778</v>
@@ -4709,21 +4828,22 @@
         <v>0</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" s="10" t="b">
+        <v>102</v>
+      </c>
+      <c r="G28" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C29" s="6" t="n">
         <v>45730.3893287037</v>
@@ -4735,21 +4855,22 @@
         <v>0</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="10" t="b">
+        <v>105</v>
+      </c>
+      <c r="G29" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30" s="6" t="n">
         <v>45707.6586805556</v>
@@ -4761,21 +4882,22 @@
         <v>0</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G30" s="10" t="b">
+        <v>108</v>
+      </c>
+      <c r="G30" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C31" s="6" t="n">
         <v>45702.025775463</v>
@@ -4787,21 +4909,22 @@
         <v>0</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G31" s="10" t="b">
+        <v>111</v>
+      </c>
+      <c r="G31" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C32" s="6" t="n">
         <v>45698.7268287037</v>
@@ -4813,21 +4936,22 @@
         <v>0</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G32" s="10" t="b">
+        <v>114</v>
+      </c>
+      <c r="G32" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C33" s="6" t="n">
         <v>45692.4376851852</v>
@@ -4839,21 +4963,22 @@
         <v>0</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="G33" s="10" t="b">
+        <v>117</v>
+      </c>
+      <c r="G33" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C34" s="6" t="n">
         <v>45692.4373263889</v>
@@ -4865,21 +4990,22 @@
         <v>0</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G34" s="10" t="b">
+        <v>120</v>
+      </c>
+      <c r="G34" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C35" s="6" t="n">
         <v>45692.4368287037</v>
@@ -4891,21 +5017,22 @@
         <v>0</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G35" s="10" t="b">
+        <v>120</v>
+      </c>
+      <c r="G35" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C36" s="6" t="n">
         <v>45691.9950231481</v>
@@ -4917,21 +5044,22 @@
         <v>0</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="G36" s="10" t="b">
+        <v>125</v>
+      </c>
+      <c r="G36" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C37" s="6" t="n">
         <v>45691.9814467593</v>
@@ -4943,21 +5071,22 @@
         <v>0</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G37" s="10" t="b">
+        <v>128</v>
+      </c>
+      <c r="G37" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C38" s="6" t="n">
         <v>45691.9681018519</v>
@@ -4969,21 +5098,22 @@
         <v>0</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G38" s="10" t="b">
+        <v>131</v>
+      </c>
+      <c r="G38" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C39" s="6" t="n">
         <v>45686.6365162037</v>
@@ -4995,21 +5125,22 @@
         <v>0</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="G39" s="10" t="b">
+        <v>134</v>
+      </c>
+      <c r="G39" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C40" s="6" t="n">
         <v>45684.3798842593</v>
@@ -5021,21 +5152,22 @@
         <v>0</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G40" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>33</v>
+        <v>137</v>
+      </c>
+      <c r="G40" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C41" s="6" t="n">
         <v>45680.7211574074</v>
@@ -5047,21 +5179,22 @@
         <v>0</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="G41" s="10" t="b">
+        <v>140</v>
+      </c>
+      <c r="G41" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C42" s="6" t="n">
         <v>45679.7208912037</v>
@@ -5073,21 +5206,22 @@
         <v>0</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="G42" s="10" t="b">
+        <v>143</v>
+      </c>
+      <c r="G42" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C43" s="6" t="n">
         <v>45674.5175</v>
@@ -5099,21 +5233,22 @@
         <v>0</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G43" s="10" t="b">
+        <v>146</v>
+      </c>
+      <c r="G43" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C44" s="6" t="n">
         <v>45674.5159953704</v>
@@ -5125,21 +5260,22 @@
         <v>0</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G44" s="10" t="b">
+        <v>149</v>
+      </c>
+      <c r="G44" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C45" s="6" t="n">
         <v>45671.5071296296</v>
@@ -5151,21 +5287,22 @@
         <v>0</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="G45" s="10" t="b">
+        <v>152</v>
+      </c>
+      <c r="G45" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C46" s="6" t="n">
         <v>45670.6857523148</v>
@@ -5177,21 +5314,22 @@
         <v>0</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="G46" s="10" t="b">
+        <v>155</v>
+      </c>
+      <c r="G46" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C47" s="6" t="n">
         <v>45660.6433101852</v>
@@ -5203,21 +5341,22 @@
         <v>0</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G47" s="10" t="b">
+        <v>158</v>
+      </c>
+      <c r="G47" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C48" s="6" t="n">
         <v>45621.6223726852</v>
@@ -5229,21 +5368,22 @@
         <v>0</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="G48" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>33</v>
+        <v>161</v>
+      </c>
+      <c r="G48" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C49" s="6" t="n">
         <v>45603.7321643519</v>
@@ -5255,21 +5395,22 @@
         <v>0</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="G49" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>33</v>
+        <v>164</v>
+      </c>
+      <c r="G49" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C50" s="6" t="n">
         <v>45603.1990625</v>
@@ -5281,21 +5422,22 @@
         <v>0</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="G50" s="10" t="b">
+        <v>167</v>
+      </c>
+      <c r="G50" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C51" s="6" t="n">
         <v>45572.5308912037</v>
@@ -5307,21 +5449,22 @@
         <v>0</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="G51" s="10" t="b">
+        <v>170</v>
+      </c>
+      <c r="G51" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C52" s="6" t="n">
         <v>45532.7298842593</v>
@@ -5333,25 +5476,25 @@
         <v>0</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G52" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C53" s="6" t="n">
         <v>45517.7053819444</v>
@@ -5363,21 +5506,22 @@
         <v>0</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="G53" s="10" t="b">
+        <v>177</v>
+      </c>
+      <c r="G53" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C54" s="6" t="n">
         <v>45506.4822800926</v>
@@ -5389,21 +5533,22 @@
         <v>0</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G54" s="10" t="b">
+        <v>180</v>
+      </c>
+      <c r="G54" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C55" s="6" t="n">
         <v>45488.2108449074</v>
@@ -5415,21 +5560,22 @@
         <v>0</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="G55" s="10" t="b">
+        <v>183</v>
+      </c>
+      <c r="G55" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C56" s="6" t="n">
         <v>45476.6756712963</v>
@@ -5441,21 +5587,22 @@
         <v>0</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="G56" s="10" t="b">
+        <v>186</v>
+      </c>
+      <c r="G56" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C57" s="6" t="n">
         <v>45449.3616319444</v>
@@ -5467,21 +5614,22 @@
         <v>0</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="G57" s="10" t="b">
+        <v>189</v>
+      </c>
+      <c r="G57" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C58" s="6" t="n">
         <v>45432.6360185185</v>
@@ -5493,21 +5641,22 @@
         <v>0</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="G58" s="10" t="b">
+        <v>192</v>
+      </c>
+      <c r="G58" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C59" s="6" t="n">
         <v>45418.3391898148</v>
@@ -5519,21 +5668,22 @@
         <v>0</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="G59" s="10" t="b">
+        <v>195</v>
+      </c>
+      <c r="G59" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C60" s="6" t="n">
         <v>45330.6774768519</v>
@@ -5545,21 +5695,22 @@
         <v>0</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="G60" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H60" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G60" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H60" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C61" s="6" t="n">
         <v>45320.6033564815</v>
@@ -5571,21 +5722,22 @@
         <v>0</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G61" s="10" t="b">
+        <v>201</v>
+      </c>
+      <c r="G61" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C62" s="6" t="n">
         <v>45320.6033101852</v>
@@ -5597,21 +5749,22 @@
         <v>0</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="G62" s="10" t="b">
+        <v>204</v>
+      </c>
+      <c r="G62" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C63" s="6" t="n">
         <v>45302.0078703704</v>
@@ -5623,21 +5776,22 @@
         <v>0</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="G63" s="10" t="b">
+        <v>207</v>
+      </c>
+      <c r="G63" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C64" s="6" t="n">
         <v>45299.6472916667</v>
@@ -5649,21 +5803,22 @@
         <v>0</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="G64" s="10" t="b">
+        <v>210</v>
+      </c>
+      <c r="G64" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C65" s="6" t="n">
         <v>45251.665162037</v>
@@ -5675,21 +5830,22 @@
         <v>0</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G65" s="10" t="b">
+        <v>213</v>
+      </c>
+      <c r="G65" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C66" s="6" t="n">
         <v>45202.5463541667</v>
@@ -5701,21 +5857,22 @@
         <v>0</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="G66" s="10" t="b">
+        <v>216</v>
+      </c>
+      <c r="G66" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C67" s="6" t="n">
         <v>45202.5430092593</v>
@@ -5727,21 +5884,22 @@
         <v>0</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G67" s="10" t="b">
+        <v>219</v>
+      </c>
+      <c r="G67" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C68" s="6" t="n">
         <v>45182.3593287037</v>
@@ -5753,21 +5911,22 @@
         <v>0</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="G68" s="10" t="b">
+        <v>222</v>
+      </c>
+      <c r="G68" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C69" s="6" t="n">
         <v>45182.3550347222</v>
@@ -5779,21 +5938,22 @@
         <v>0</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="G69" s="10" t="b">
+        <v>225</v>
+      </c>
+      <c r="G69" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C70" s="6" t="n">
         <v>45182.3533680556</v>
@@ -5805,21 +5965,22 @@
         <v>0</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G70" s="10" t="b">
+        <v>228</v>
+      </c>
+      <c r="G70" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C71" s="6" t="n">
         <v>45182.3515277778</v>
@@ -5831,21 +5992,22 @@
         <v>0</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="G71" s="10" t="b">
+        <v>231</v>
+      </c>
+      <c r="G71" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C72" s="6" t="n">
         <v>45169.3461689815</v>
@@ -5857,21 +6019,22 @@
         <v>0</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="G72" s="10" t="b">
+        <v>234</v>
+      </c>
+      <c r="G72" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C73" s="6" t="n">
         <v>45169.3456828704</v>
@@ -5883,21 +6046,22 @@
         <v>0</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="G73" s="10" t="b">
+        <v>237</v>
+      </c>
+      <c r="G73" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C74" s="6" t="n">
         <v>45154.009212963</v>
@@ -5909,21 +6073,22 @@
         <v>0</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="G74" s="10" t="b">
+        <v>240</v>
+      </c>
+      <c r="G74" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C75" s="6" t="n">
         <v>45136.8341666667</v>
@@ -5935,21 +6100,22 @@
         <v>0</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="G75" s="10" t="b">
+        <v>243</v>
+      </c>
+      <c r="G75" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C76" s="6" t="n">
         <v>45136.832337963</v>
@@ -5961,21 +6127,22 @@
         <v>0</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="G76" s="10" t="b">
+        <v>246</v>
+      </c>
+      <c r="G76" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C77" s="6" t="n">
         <v>45136.8287847222</v>
@@ -5987,21 +6154,22 @@
         <v>0</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G77" s="10" t="b">
+        <v>249</v>
+      </c>
+      <c r="G77" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C78" s="6" t="n">
         <v>45043.494375</v>
@@ -6013,21 +6181,22 @@
         <v>0</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="G78" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H78" s="11" t="s">
-        <v>33</v>
+        <v>252</v>
+      </c>
+      <c r="G78" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C79" s="6" t="n">
         <v>45014.8957638889</v>
@@ -6039,21 +6208,22 @@
         <v>0</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="G79" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H79" s="11" t="s">
-        <v>33</v>
+        <v>255</v>
+      </c>
+      <c r="G79" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C80" s="6" t="n">
         <v>45014.7074884259</v>
@@ -6065,23 +6235,23 @@
         <v>0</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G80" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H80" s="11" t="s">
+      <c r="H80" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I80" s="5"/>
     </row>
     <row r="81" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C81" s="6" t="n">
         <v>45009.6759953704</v>
@@ -6093,21 +6263,22 @@
         <v>0</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="G81" s="10" t="b">
+        <v>261</v>
+      </c>
+      <c r="G81" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C82" s="6" t="n">
         <v>44991.8924189815</v>
@@ -6119,21 +6290,22 @@
         <v>0</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="G82" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H82" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="G82" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H82" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C83" s="6" t="n">
         <v>44970.9496412037</v>
@@ -6145,21 +6317,22 @@
         <v>0</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="G83" s="10" t="b">
+        <v>267</v>
+      </c>
+      <c r="G83" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C84" s="6" t="n">
         <v>44966.7852430556</v>
@@ -6171,25 +6344,25 @@
         <v>0</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G84" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I84" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C85" s="6" t="n">
         <v>44966.757337963</v>
@@ -6201,21 +6374,22 @@
         <v>0</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="G85" s="10" t="b">
+        <v>275</v>
+      </c>
+      <c r="G85" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C86" s="6" t="n">
         <v>44960.7653240741</v>
@@ -6227,21 +6401,22 @@
         <v>0</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="G86" s="10" t="b">
+        <v>278</v>
+      </c>
+      <c r="G86" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C87" s="6" t="n">
         <v>44952.5041435185</v>
@@ -6253,21 +6428,22 @@
         <v>0</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="G87" s="10" t="b">
+        <v>281</v>
+      </c>
+      <c r="G87" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C88" s="6" t="n">
         <v>44894.8211458333</v>
@@ -6279,21 +6455,22 @@
         <v>0</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="G88" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H88" s="11" t="s">
-        <v>33</v>
+        <v>284</v>
+      </c>
+      <c r="G88" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C89" s="6" t="n">
         <v>44875.8107060185</v>
@@ -6305,21 +6482,22 @@
         <v>0</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="G89" s="10" t="b">
+        <v>287</v>
+      </c>
+      <c r="G89" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C90" s="6" t="n">
         <v>44812.7771296296</v>
@@ -6331,21 +6509,22 @@
         <v>0</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="G90" s="10" t="b">
+        <v>290</v>
+      </c>
+      <c r="G90" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C91" s="6" t="n">
         <v>44812.7208912037</v>
@@ -6357,21 +6536,22 @@
         <v>0</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="G91" s="10" t="b">
+        <v>293</v>
+      </c>
+      <c r="G91" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C92" s="6" t="n">
         <v>44805.8982638889</v>
@@ -6383,21 +6563,22 @@
         <v>0</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="G92" s="10" t="b">
+        <v>296</v>
+      </c>
+      <c r="G92" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H92" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C93" s="6" t="n">
         <v>44799.6221180556</v>
@@ -6409,25 +6590,25 @@
         <v>0</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G93" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I93" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C94" s="6" t="n">
         <v>44760.6952430556</v>
@@ -6439,25 +6620,25 @@
         <v>0</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G94" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I94" s="9" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C95" s="6" t="n">
         <v>44713.8200694444</v>
@@ -6469,21 +6650,22 @@
         <v>0</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="G95" s="10" t="b">
+        <v>307</v>
+      </c>
+      <c r="G95" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H95" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C96" s="6" t="n">
         <v>44503.2003703704</v>
@@ -6495,25 +6677,25 @@
         <v>0</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G96" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I96" s="9" t="s">
-        <v>61</v>
+        <v>46</v>
+      </c>
+      <c r="I96" s="10" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C97" s="6" t="n">
         <v>44454.7181134259</v>
@@ -6525,25 +6707,25 @@
         <v>0</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G97" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="I97" s="9" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C98" s="6" t="n">
         <v>44427.9998148148</v>
@@ -6555,21 +6737,22 @@
         <v>0</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="G98" s="10" t="b">
+        <v>319</v>
+      </c>
+      <c r="G98" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C99" s="6" t="n">
         <v>44378.0131365741</v>
@@ -6581,21 +6764,22 @@
         <v>0</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="G99" s="10" t="b">
+        <v>322</v>
+      </c>
+      <c r="G99" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C100" s="6" t="n">
         <v>44329.152650463</v>
@@ -6607,22 +6791,22 @@
         <v>0</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G100" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H100" s="11" t="s">
+      <c r="H100" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C101" s="6" t="n">
         <v>44296.1468287037</v>
@@ -6634,21 +6818,22 @@
         <v>0</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="G101" s="10" t="b">
+        <v>328</v>
+      </c>
+      <c r="G101" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H101" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C102" s="6" t="n">
         <v>44237.7602662037</v>
@@ -6660,21 +6845,22 @@
         <v>0</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="G102" s="10" t="b">
+        <v>331</v>
+      </c>
+      <c r="G102" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C103" s="6" t="n">
         <v>44181.7227546296</v>
@@ -6686,21 +6872,22 @@
         <v>0</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="G103" s="10" t="b">
+        <v>334</v>
+      </c>
+      <c r="G103" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H103" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C104" s="6" t="n">
         <v>44176.7845833333</v>
@@ -6712,21 +6899,22 @@
         <v>0</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="G104" s="10" t="b">
+        <v>337</v>
+      </c>
+      <c r="G104" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C105" s="6" t="n">
         <v>44082.9717592593</v>
@@ -6738,21 +6926,22 @@
         <v>0</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="G105" s="10" t="b">
+        <v>340</v>
+      </c>
+      <c r="G105" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C106" s="6" t="n">
         <v>44082.9704050926</v>
@@ -6764,21 +6953,22 @@
         <v>0</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="G106" s="10" t="b">
+        <v>343</v>
+      </c>
+      <c r="G106" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C107" s="6" t="n">
         <v>44049.5190509259</v>
@@ -6790,21 +6980,22 @@
         <v>0</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="G107" s="10" t="b">
+        <v>346</v>
+      </c>
+      <c r="G107" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C108" s="6" t="n">
         <v>43989.8130208333</v>
@@ -6816,21 +7007,22 @@
         <v>0</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="G108" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H108" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="G108" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H108" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C109" s="6" t="n">
         <v>43954.6611226852</v>
@@ -6842,21 +7034,22 @@
         <v>0</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="G109" s="10" t="b">
+        <v>352</v>
+      </c>
+      <c r="G109" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="4" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C110" s="6" t="n">
         <v>43934.8656018519</v>
@@ -6868,21 +7061,22 @@
         <v>0</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="G110" s="10" t="b">
+        <v>355</v>
+      </c>
+      <c r="G110" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C111" s="6" t="n">
         <v>43924.7954398148</v>
@@ -6894,25 +7088,25 @@
         <v>0</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G111" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I111" s="9" t="s">
-        <v>357</v>
+        <v>46</v>
+      </c>
+      <c r="I111" s="10" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="4" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C112" s="6" t="n">
         <v>43867.7611111111</v>
@@ -6924,21 +7118,22 @@
         <v>0</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="G112" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H112" s="11" t="s">
-        <v>33</v>
+        <v>362</v>
+      </c>
+      <c r="G112" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H112" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C113" s="6" t="n">
         <v>43866.9327662037</v>
@@ -6950,14 +7145,14 @@
         <v>0</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="G113" s="8" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H113" s="11" t="s">
-        <v>33</v>
+      <c r="H113" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -7094,8 +7289,8 @@
   </sheetPr>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="90" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7108,46 +7303,46 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="255"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="68.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="142.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C2" s="14" t="n">
+        <v>367</v>
+      </c>
+      <c r="C2" s="13" t="n">
         <v>45610.2021643519</v>
       </c>
       <c r="D2" s="1" t="n">
@@ -7156,25 +7351,25 @@
       <c r="E2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="G2" s="16" t="n">
+      <c r="F2" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="G2" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C3" s="14" t="n">
+        <v>371</v>
+      </c>
+      <c r="C3" s="13" t="n">
         <v>44602.6183680556</v>
       </c>
       <c r="D3" s="1" t="n">
@@ -7183,25 +7378,25 @@
       <c r="E3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="G3" s="16" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>367</v>
+      <c r="F3" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G3" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C4" s="14" t="n">
+        <v>374</v>
+      </c>
+      <c r="C4" s="13" t="n">
         <v>45043.3846064815</v>
       </c>
       <c r="D4" s="1" t="n">
@@ -7210,28 +7405,28 @@
       <c r="E4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="G4" s="16" t="n">
+      <c r="F4" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="G4" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="C5" s="14" t="n">
+        <v>378</v>
+      </c>
+      <c r="C5" s="13" t="n">
         <v>45582.5868518519</v>
       </c>
       <c r="D5" s="1" t="n">
@@ -7240,25 +7435,25 @@
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="G5" s="16" t="n">
+      <c r="F5" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="G5" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C6" s="14" t="n">
+        <v>381</v>
+      </c>
+      <c r="C6" s="13" t="n">
         <v>45237.4165046296</v>
       </c>
       <c r="D6" s="1" t="n">
@@ -7267,28 +7462,28 @@
       <c r="E6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="G6" s="16" t="n">
+      <c r="F6" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="G6" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C7" s="14" t="n">
+        <v>385</v>
+      </c>
+      <c r="C7" s="13" t="n">
         <v>45023.8305439815</v>
       </c>
       <c r="D7" s="1" t="n">
@@ -7297,25 +7492,25 @@
       <c r="E7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="G7" s="16" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>367</v>
+      <c r="F7" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="G7" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="C8" s="14" t="n">
+        <v>388</v>
+      </c>
+      <c r="C8" s="13" t="n">
         <v>45723.9116435185</v>
       </c>
       <c r="D8" s="1" t="n">
@@ -7324,25 +7519,25 @@
       <c r="E8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>387</v>
-      </c>
-      <c r="G8" s="16" t="n">
+      <c r="F8" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="G8" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C9" s="14" t="n">
+        <v>391</v>
+      </c>
+      <c r="C9" s="13" t="n">
         <v>45708.4314583333</v>
       </c>
       <c r="D9" s="1" t="n">
@@ -7351,25 +7546,25 @@
       <c r="E9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>390</v>
-      </c>
-      <c r="G9" s="16" t="n">
+      <c r="F9" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="G9" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="C10" s="14" t="n">
+        <v>394</v>
+      </c>
+      <c r="C10" s="13" t="n">
         <v>45708.1901736111</v>
       </c>
       <c r="D10" s="1" t="n">
@@ -7378,25 +7573,25 @@
       <c r="E10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>393</v>
-      </c>
-      <c r="G10" s="16" t="n">
+      <c r="F10" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="G10" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C11" s="14" t="n">
+        <v>397</v>
+      </c>
+      <c r="C11" s="13" t="n">
         <v>45708.1896180556</v>
       </c>
       <c r="D11" s="1" t="n">
@@ -7405,25 +7600,25 @@
       <c r="E11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="G11" s="16" t="n">
+      <c r="F11" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="G11" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="C12" s="14" t="n">
+        <v>400</v>
+      </c>
+      <c r="C12" s="13" t="n">
         <v>45708.1891087963</v>
       </c>
       <c r="D12" s="1" t="n">
@@ -7432,25 +7627,25 @@
       <c r="E12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="15" t="s">
-        <v>399</v>
-      </c>
-      <c r="G12" s="16" t="n">
+      <c r="F12" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="G12" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C13" s="14" t="n">
+        <v>403</v>
+      </c>
+      <c r="C13" s="13" t="n">
         <v>45707.6379861111</v>
       </c>
       <c r="D13" s="1" t="n">
@@ -7459,25 +7654,25 @@
       <c r="E13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>402</v>
-      </c>
-      <c r="G13" s="16" t="n">
+      <c r="F13" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="G13" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C14" s="14" t="n">
+        <v>406</v>
+      </c>
+      <c r="C14" s="13" t="n">
         <v>45707.4038541667</v>
       </c>
       <c r="D14" s="1" t="n">
@@ -7486,25 +7681,25 @@
       <c r="E14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="15" t="s">
-        <v>405</v>
-      </c>
-      <c r="G14" s="16" t="n">
+      <c r="F14" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="G14" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="C15" s="14" t="n">
+        <v>409</v>
+      </c>
+      <c r="C15" s="13" t="n">
         <v>45630.6213541667</v>
       </c>
       <c r="D15" s="1" t="n">
@@ -7513,25 +7708,25 @@
       <c r="E15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>408</v>
-      </c>
-      <c r="G15" s="16" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>367</v>
+      <c r="F15" s="14" t="s">
+        <v>410</v>
+      </c>
+      <c r="G15" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C16" s="14" t="n">
+        <v>412</v>
+      </c>
+      <c r="C16" s="13" t="n">
         <v>45617.6777430556</v>
       </c>
       <c r="D16" s="1" t="n">
@@ -7540,25 +7735,25 @@
       <c r="E16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>411</v>
-      </c>
-      <c r="G16" s="16" t="n">
+      <c r="F16" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="G16" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C17" s="14" t="n">
+        <v>415</v>
+      </c>
+      <c r="C17" s="13" t="n">
         <v>45612.0007175926</v>
       </c>
       <c r="D17" s="1" t="n">
@@ -7567,25 +7762,25 @@
       <c r="E17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>414</v>
-      </c>
-      <c r="G17" s="16" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>367</v>
+      <c r="F17" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="G17" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C18" s="14" t="n">
+        <v>418</v>
+      </c>
+      <c r="C18" s="13" t="n">
         <v>45608.6264930556</v>
       </c>
       <c r="D18" s="1" t="n">
@@ -7595,24 +7790,24 @@
         <v>0</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>417</v>
-      </c>
-      <c r="G18" s="16" t="n">
+        <v>419</v>
+      </c>
+      <c r="G18" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C19" s="14" t="n">
+        <v>421</v>
+      </c>
+      <c r="C19" s="13" t="n">
         <v>45544.4907638889</v>
       </c>
       <c r="D19" s="1" t="n">
@@ -7621,25 +7816,25 @@
       <c r="E19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>420</v>
-      </c>
-      <c r="G19" s="16" t="n">
+      <c r="F19" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="G19" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="C20" s="14" t="n">
+        <v>424</v>
+      </c>
+      <c r="C20" s="13" t="n">
         <v>45464.7875578704</v>
       </c>
       <c r="D20" s="1" t="n">
@@ -7648,25 +7843,25 @@
       <c r="E20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>423</v>
-      </c>
-      <c r="G20" s="16" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>367</v>
+      <c r="F20" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="G20" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="C21" s="14" t="n">
+        <v>427</v>
+      </c>
+      <c r="C21" s="13" t="n">
         <v>45169.3445949074</v>
       </c>
       <c r="D21" s="1" t="n">
@@ -7676,24 +7871,24 @@
         <v>0</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>426</v>
-      </c>
-      <c r="G21" s="16" t="n">
+        <v>428</v>
+      </c>
+      <c r="G21" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C22" s="14" t="n">
+        <v>430</v>
+      </c>
+      <c r="C22" s="13" t="n">
         <v>45162.5534259259</v>
       </c>
       <c r="D22" s="1" t="n">
@@ -7702,25 +7897,25 @@
       <c r="E22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>429</v>
-      </c>
-      <c r="G22" s="16" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>367</v>
+      <c r="F22" s="14" t="s">
+        <v>431</v>
+      </c>
+      <c r="G22" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C23" s="14" t="n">
+        <v>433</v>
+      </c>
+      <c r="C23" s="13" t="n">
         <v>45131.3296990741</v>
       </c>
       <c r="D23" s="1" t="n">
@@ -7729,25 +7924,25 @@
       <c r="E23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>432</v>
-      </c>
-      <c r="G23" s="16" t="n">
+      <c r="F23" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="G23" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C24" s="14" t="n">
+        <v>436</v>
+      </c>
+      <c r="C24" s="13" t="n">
         <v>45110.506400463</v>
       </c>
       <c r="D24" s="1" t="n">
@@ -7756,28 +7951,28 @@
       <c r="E24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="G24" s="16" t="n">
+      <c r="F24" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="G24" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C25" s="14" t="n">
+        <v>440</v>
+      </c>
+      <c r="C25" s="13" t="n">
         <v>45065.9196180556</v>
       </c>
       <c r="D25" s="1" t="n">
@@ -7786,28 +7981,28 @@
       <c r="E25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>439</v>
-      </c>
-      <c r="G25" s="16" t="n">
+      <c r="F25" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="G25" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C26" s="14" t="n">
+        <v>445</v>
+      </c>
+      <c r="C26" s="13" t="n">
         <v>44960.6602430556</v>
       </c>
       <c r="D26" s="1" t="n">
@@ -7816,28 +8011,28 @@
       <c r="E26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F26" s="15" t="s">
-        <v>444</v>
-      </c>
-      <c r="G26" s="16" t="n">
+      <c r="F26" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="G26" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>445</v>
+        <v>46</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="C27" s="14" t="n">
+        <v>449</v>
+      </c>
+      <c r="C27" s="13" t="n">
         <v>44865.3693634259</v>
       </c>
       <c r="D27" s="1" t="n">
@@ -7846,25 +8041,25 @@
       <c r="E27" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F27" s="15" t="s">
-        <v>448</v>
-      </c>
-      <c r="G27" s="16" t="n">
+      <c r="F27" s="14" t="s">
+        <v>450</v>
+      </c>
+      <c r="G27" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="C28" s="14" t="n">
+        <v>452</v>
+      </c>
+      <c r="C28" s="13" t="n">
         <v>44818.6455555556</v>
       </c>
       <c r="D28" s="1" t="n">
@@ -7873,25 +8068,25 @@
       <c r="E28" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F28" s="15" t="s">
-        <v>451</v>
-      </c>
-      <c r="G28" s="16" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>367</v>
+      <c r="F28" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="G28" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="C29" s="14" t="n">
+        <v>455</v>
+      </c>
+      <c r="C29" s="13" t="n">
         <v>44787.841712963</v>
       </c>
       <c r="D29" s="1" t="n">
@@ -7900,28 +8095,28 @@
       <c r="E29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F29" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="G29" s="16" t="n">
+      <c r="F29" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="G29" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="C30" s="14" t="n">
+        <v>459</v>
+      </c>
+      <c r="C30" s="13" t="n">
         <v>44557.8673263889</v>
       </c>
       <c r="D30" s="1" t="n">
@@ -7930,28 +8125,28 @@
       <c r="E30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F30" s="15" t="s">
-        <v>458</v>
-      </c>
-      <c r="G30" s="16" t="n">
+      <c r="F30" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="G30" s="15" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="C31" s="14" t="n">
+        <v>463</v>
+      </c>
+      <c r="C31" s="13" t="n">
         <v>44455.7410416667</v>
       </c>
       <c r="D31" s="1" t="n">
@@ -7960,25 +8155,25 @@
       <c r="E31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F31" s="15" t="s">
-        <v>462</v>
-      </c>
-      <c r="G31" s="16" t="n">
+      <c r="F31" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="G31" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="C32" s="14" t="n">
+        <v>466</v>
+      </c>
+      <c r="C32" s="13" t="n">
         <v>44385.8234722222</v>
       </c>
       <c r="D32" s="1" t="n">
@@ -7987,25 +8182,25 @@
       <c r="E32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>465</v>
-      </c>
-      <c r="G32" s="16" t="n">
+      <c r="F32" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="G32" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="C33" s="14" t="n">
+        <v>469</v>
+      </c>
+      <c r="C33" s="13" t="n">
         <v>44285.6562962963</v>
       </c>
       <c r="D33" s="1" t="n">
@@ -8014,25 +8209,25 @@
       <c r="E33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>468</v>
-      </c>
-      <c r="G33" s="16" t="n">
+      <c r="F33" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="G33" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="C34" s="14" t="n">
+        <v>472</v>
+      </c>
+      <c r="C34" s="13" t="n">
         <v>44011.4896296296</v>
       </c>
       <c r="D34" s="1" t="n">
@@ -8041,15 +8236,15 @@
       <c r="E34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>471</v>
-      </c>
-      <c r="G34" s="16" t="n">
+      <c r="F34" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="G34" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -8107,8 +8302,8 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="90" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8150,16 +8345,16 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>472</v>
+      <c r="A2" s="11" t="s">
+        <v>474</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>45377.6785069444</v>
@@ -8171,21 +8366,22 @@
         <v>0</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="G2" s="8" t="b">
+        <v>476</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C3" s="6" t="n">
         <v>45377.6762037037</v>
@@ -8197,17 +8393,17 @@
         <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="G3" s="8" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>12</v>
+        <v>480</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>